<commit_message>
testes de alteração de chave em json
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\OneDrive\Área de Trabalho\BigDataPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F688268-9AF3-4E05-BDA8-49FC3257E2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5207A2C-5CFF-4332-BFCC-D712E2C44D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{01698FFF-0B9D-4444-8B58-7D9A3F4ED84F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{01698FFF-0B9D-4444-8B58-7D9A3F4ED84F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,71 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Célula 1</t>
-  </si>
-  <si>
-    <t>Célula 2</t>
-  </si>
-  <si>
-    <t>Célula 3</t>
-  </si>
-  <si>
-    <t>Célula 4</t>
-  </si>
-  <si>
-    <t>Célula 5</t>
-  </si>
-  <si>
-    <t>Célula 6</t>
-  </si>
-  <si>
-    <t>Célula 7</t>
-  </si>
-  <si>
-    <t>Célula 8</t>
-  </si>
-  <si>
-    <t>Coluna 1</t>
-  </si>
-  <si>
-    <t>Coluna 2</t>
-  </si>
-  <si>
-    <t>Coluna 3</t>
-  </si>
-  <si>
-    <t>Célula 9</t>
-  </si>
-  <si>
-    <t>Célula 10</t>
-  </si>
-  <si>
-    <t>Célula 11</t>
-  </si>
-  <si>
-    <t>Célula 12</t>
-  </si>
-  <si>
-    <t>Célula 13</t>
-  </si>
-  <si>
-    <t>Célula 14</t>
-  </si>
-  <si>
-    <t>Célula 15</t>
-  </si>
-  <si>
-    <t>Célula 16</t>
-  </si>
-  <si>
-    <t>Célula 17</t>
-  </si>
-  <si>
-    <t>Célula 18</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -121,7 +57,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <u/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -130,15 +75,8 @@
     </font>
     <font>
       <i/>
+      <u/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -203,15 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -221,7 +151,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E6E586-A15C-4ADE-A795-77010672502E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,81 +508,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="A1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -657,12 +553,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758EF185-9E7B-48D7-A358-2D60BDC6D844}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
+      <c r="A1" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>